<commit_message>
Update Add Bobbin Weigth to Remain Tag
</commit_message>
<xml_diff>
--- a/bin/Debug/Template/RemainingTagTemplate.xlsx
+++ b/bin/Debug/Template/RemainingTagTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Project\My C# project\MachineDeptApp\MachineDeptApp v1.0.0.8\bin\Debug\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Works\MC-Dept-App\bin\Debug\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84FDFDA-C103-4F3C-99BE-18766E066DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13E174C-9040-40B1-85F4-5DCE699D0676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{2B55643B-660D-486C-B673-E46BBE604A86}"/>
+    <workbookView xWindow="6915" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{2B55643B-660D-486C-B673-E46BBE604A86}"/>
   </bookViews>
   <sheets>
     <sheet name="RachhanSystem" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Code</t>
   </si>
@@ -65,6 +65,18 @@
   </si>
   <si>
     <t>ចំនួននៅសល់សរុប</t>
+  </si>
+  <si>
+    <t>UL1061-22 GRN  (17/0.16)(SD)</t>
+  </si>
+  <si>
+    <t>Shindin</t>
+  </si>
+  <si>
+    <t>3,050 m</t>
+  </si>
+  <si>
+    <t>3,050 m ( 13 KG )</t>
   </si>
 </sst>
 </file>
@@ -577,10 +589,12 @@
       <c r="B1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6"/>
+      <c r="C1" s="6">
+        <v>3218</v>
+      </c>
       <c r="D1" s="7" t="str">
         <f>"*"&amp;C1&amp;"*"</f>
-        <v>**</v>
+        <v>*3218*</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -590,7 +604,9 @@
       <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="15"/>
+      <c r="C2" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="D2" s="15"/>
     </row>
     <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="1">
@@ -600,7 +616,9 @@
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="16"/>
+      <c r="C3" s="16" t="s">
+        <v>13</v>
+      </c>
       <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" ht="31.5" x14ac:dyDescent="1">
@@ -610,7 +628,9 @@
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="16"/>
+      <c r="C4" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:4" ht="39.75" x14ac:dyDescent="0.25">
@@ -620,7 +640,9 @@
       <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="1:4" ht="31.5" x14ac:dyDescent="1">
@@ -640,7 +662,9 @@
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="14">
+        <v>45682.420115740744</v>
+      </c>
       <c r="D7" s="14"/>
     </row>
   </sheetData>

</xml_diff>